<commit_message>
Add tests to Total_Risk macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/_test_results.xlsx
+++ b/Performance Analytics Library/_test_results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="248">
   <si>
     <t>test</t>
   </si>
@@ -749,6 +749,18 @@
   </si>
   <si>
     <t>Test Specific Risk for yearly returns</t>
+  </si>
+  <si>
+    <t>Total_Risk1</t>
+  </si>
+  <si>
+    <t>Test Total Risk with VARDEF=DF</t>
+  </si>
+  <si>
+    <t>Total_Risk2</t>
+  </si>
+  <si>
+    <t>Test Total Risk with VARDEF=N</t>
   </si>
 </sst>
 </file>
@@ -1108,10 +1120,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>

</xml_diff>